<commit_message>
Connection to authentication server from chat server now works, can send login and register information
</commit_message>
<xml_diff>
--- a/Command IDs.xlsx
+++ b/Command IDs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Desktop\INFO - 6016\Projects\1\NetworkProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cryst\Downloads\Networking\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Command ID</t>
   </si>
@@ -54,6 +54,24 @@
   </si>
   <si>
     <t>Message others in Room</t>
+  </si>
+  <si>
+    <t>PROJECT 2</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Server Receive</t>
+  </si>
+  <si>
+    <t>Server Send</t>
+  </si>
+  <si>
+    <t>Authentication</t>
   </si>
 </sst>
 </file>
@@ -371,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,9 +400,11 @@
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -395,7 +415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -403,7 +423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -414,7 +434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -425,7 +445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -436,7 +456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -447,9 +467,92 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited proto, added authentication server responses to chat server
</commit_message>
<xml_diff>
--- a/Command IDs.xlsx
+++ b/Command IDs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Command ID</t>
   </si>
@@ -65,13 +65,31 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Server Receive</t>
-  </si>
-  <si>
-    <t>Server Send</t>
-  </si>
-  <si>
     <t>Authentication</t>
+  </si>
+  <si>
+    <t>Register Success</t>
+  </si>
+  <si>
+    <t>Login Success</t>
+  </si>
+  <si>
+    <t>Register Failure</t>
+  </si>
+  <si>
+    <t>Login Failure</t>
+  </si>
+  <si>
+    <t>RequestId=client index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server </t>
+  </si>
+  <si>
+    <t>Register/Login Success</t>
+  </si>
+  <si>
+    <t>Register/Login Failure</t>
   </si>
 </sst>
 </file>
@@ -389,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="166" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,8 +418,8 @@
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -476,6 +494,9 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -485,13 +506,13 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -507,6 +528,9 @@
       <c r="E12" t="s">
         <v>11</v>
       </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -521,6 +545,9 @@
       <c r="E13" t="s">
         <v>12</v>
       </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -532,6 +559,9 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -543,6 +573,9 @@
       <c r="D15" t="s">
         <v>7</v>
       </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -553,6 +586,32 @@
       </c>
       <c r="D16" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>